<commit_message>
login and account creation integration
</commit_message>
<xml_diff>
--- a/TcpServer/bin/Debug/net8.0/logs.xlsx
+++ b/TcpServer/bin/Debug/net8.0/logs.xlsx
@@ -105,6 +105,435 @@
   </x:si>
   <x:si>
     <x:t>2024 March 29 3:18:44 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:50:56 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:50:57 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:52:16 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:52:18 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:53:54 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:53:55 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:54:35 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:54:36 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:55:04 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:55:05 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:55:30 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 3:55:32 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:04:46 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:04:48 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:30:05 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:30:06 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:30:43 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:30:45 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:34:45 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:34:47 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:34:54 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:35:48 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:35:50 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:35:56 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:36:20 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:36:22 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:36:45 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:37:37 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:37:39 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:38:20 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:38:21 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:39:09 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:39:10 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:39:17 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:40:09 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:40:11 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:40:15 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:41:11 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:41:13 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:41:52 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:41:54 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:43:59 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:44:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:44:07 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:48:47 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:48:49 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:48:54 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:51:54 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:51:56 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:52:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:53:30 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:53:32 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:53:36 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:54:28 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:54:30 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:54:35 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:56:43 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:56:45 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:56:49 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:56:53 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:59:42 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 4:59:44 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:05:45 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:05:47 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:05:58 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:06:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:06:10 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:39:10 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:39:12 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:39:18 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:39:22 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:39:31 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:58:04 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:58:06 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:59:12 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 5:59:14 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:00:07 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:00:09 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:01:46 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:01:48 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:05:47 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:05:49 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:07:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:07:02 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:08:32 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:08:35 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:11:49 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:11:51 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:12:27 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:12:30 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:12:38 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:13:48 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:13:51 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:18:33 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:18:36 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:20:22 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:20:25 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:20:57 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:20:59 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:21:04 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:21:16 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:21:29 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:23:20 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:23:23 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:28:15 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:28:18 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:28:26 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:28:32 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Acc Signal Recieved</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:51:49 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:51:52 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:51:59 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:52:53 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:52:55 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:53:05 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:54:12 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:54:14 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 6:54:22 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:02:10 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:02:14 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:03:21 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:03:24 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:03:31 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:06:45 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:06:48 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:07:34 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:07:37 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:10:18 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:10:21 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:10:57 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:11:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:12:32 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:12:35 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:12:44 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:13:41 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:13:44 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:15:02 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:15:05 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:15:13 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:15:18 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:19:55 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:19:59 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 7:20:14 AM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -683,6 +1112,1568 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
+    <x:row r="19">
+      <x:c r="A19" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B19" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C19" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20">
+      <x:c r="A20" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B20" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C20" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21">
+      <x:c r="A21" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B21" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C21" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22">
+      <x:c r="A22" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B22" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C22" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23">
+      <x:c r="A23" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B23" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C23" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24">
+      <x:c r="A24" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B24" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C24" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25">
+      <x:c r="A25" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B25" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C25" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26">
+      <x:c r="A26" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B26" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C26" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27">
+      <x:c r="A27" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B27" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C27" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28">
+      <x:c r="A28" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B28" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C28" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29">
+      <x:c r="A29" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B29" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C29" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30">
+      <x:c r="A30" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B30" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C30" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31">
+      <x:c r="A31" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B31" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C31" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32">
+      <x:c r="A32" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B32" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C32" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33">
+      <x:c r="A33" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B33" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C33" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34">
+      <x:c r="A34" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B34" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C34" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35">
+      <x:c r="A35" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B35" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C35" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36">
+      <x:c r="A36" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B36" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C36" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37">
+      <x:c r="A37" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B37" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C37" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38">
+      <x:c r="A38" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B38" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C38" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39">
+      <x:c r="A39" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B39" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C39" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40">
+      <x:c r="A40" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B40" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C40" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41">
+      <x:c r="A41" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B41" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C41" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42">
+      <x:c r="A42" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B42" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C42" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43">
+      <x:c r="A43" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B43" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C43" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44">
+      <x:c r="A44" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B44" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C44" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45">
+      <x:c r="A45" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B45" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C45" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46">
+      <x:c r="A46" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B46" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C46" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47">
+      <x:c r="A47" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B47" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C47" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48">
+      <x:c r="A48" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B48" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C48" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49">
+      <x:c r="A49" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B49" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C49" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50">
+      <x:c r="A50" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B50" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C50" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51">
+      <x:c r="A51" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B51" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C51" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52">
+      <x:c r="A52" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B52" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C52" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53">
+      <x:c r="A53" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B53" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C53" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54">
+      <x:c r="A54" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B54" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C54" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55">
+      <x:c r="A55" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B55" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C55" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56">
+      <x:c r="A56" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B56" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C56" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57">
+      <x:c r="A57" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B57" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C57" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58">
+      <x:c r="A58" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B58" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C58" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59">
+      <x:c r="A59" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B59" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C59" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60">
+      <x:c r="A60" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B60" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C60" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61">
+      <x:c r="A61" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B61" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C61" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62">
+      <x:c r="A62" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B62" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C62" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63">
+      <x:c r="A63" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B63" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C63" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64">
+      <x:c r="A64" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B64" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C64" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65">
+      <x:c r="A65" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B65" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C65" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66">
+      <x:c r="A66" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B66" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C66" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67">
+      <x:c r="A67" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B67" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C67" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68">
+      <x:c r="A68" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B68" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C68" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69">
+      <x:c r="A69" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B69" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C69" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70">
+      <x:c r="A70" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B70" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C70" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71">
+      <x:c r="A71" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="B71" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C71" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72">
+      <x:c r="A72" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B72" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C72" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73">
+      <x:c r="A73" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B73" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C73" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74">
+      <x:c r="A74" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B74" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C74" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75">
+      <x:c r="A75" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="B75" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C75" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76">
+      <x:c r="A76" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B76" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C76" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77">
+      <x:c r="A77" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="B77" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C77" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78">
+      <x:c r="A78" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B78" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C78" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79">
+      <x:c r="A79" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B79" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C79" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80">
+      <x:c r="A80" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B80" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C80" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81">
+      <x:c r="A81" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B81" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C81" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82">
+      <x:c r="A82" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B82" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C82" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83">
+      <x:c r="A83" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B83" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C83" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84">
+      <x:c r="A84" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B84" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C84" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85">
+      <x:c r="A85" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B85" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C85" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86">
+      <x:c r="A86" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B86" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C86" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87">
+      <x:c r="A87" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B87" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C87" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88">
+      <x:c r="A88" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B88" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C88" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89">
+      <x:c r="A89" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B89" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C89" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90">
+      <x:c r="A90" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B90" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C90" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91">
+      <x:c r="A91" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B91" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C91" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92">
+      <x:c r="A92" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B92" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C92" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93">
+      <x:c r="A93" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B93" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C93" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94">
+      <x:c r="A94" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B94" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C94" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95">
+      <x:c r="A95" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B95" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C95" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96">
+      <x:c r="A96" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B96" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C96" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97">
+      <x:c r="A97" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B97" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C97" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98">
+      <x:c r="A98" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B98" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C98" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99">
+      <x:c r="A99" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B99" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C99" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100">
+      <x:c r="A100" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B100" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C100" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101">
+      <x:c r="A101" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B101" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C101" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102">
+      <x:c r="A102" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B102" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C102" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103">
+      <x:c r="A103" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B103" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C103" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104">
+      <x:c r="A104" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B104" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C104" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105">
+      <x:c r="A105" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B105" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C105" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106">
+      <x:c r="A106" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B106" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C106" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107">
+      <x:c r="A107" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="B107" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C107" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108">
+      <x:c r="A108" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="B108" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C108" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109">
+      <x:c r="A109" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="B109" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C109" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110">
+      <x:c r="A110" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B110" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C110" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111">
+      <x:c r="A111" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="B111" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C111" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112">
+      <x:c r="A112" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B112" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C112" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113">
+      <x:c r="A113" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="B113" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C113" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114">
+      <x:c r="A114" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B114" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C114" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115">
+      <x:c r="A115" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B115" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C115" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116">
+      <x:c r="A116" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="B116" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C116" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117">
+      <x:c r="A117" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="B117" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C117" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118">
+      <x:c r="A118" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="B118" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C118" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119">
+      <x:c r="A119" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B119" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C119" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120">
+      <x:c r="A120" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="B120" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C120" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121">
+      <x:c r="A121" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="B121" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C121" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="122">
+      <x:c r="A122" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B122" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C122" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123">
+      <x:c r="A123" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="B123" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C123" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124">
+      <x:c r="A124" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="B124" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C124" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125">
+      <x:c r="A125" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="B125" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C125" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126">
+      <x:c r="A126" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="B126" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C126" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127">
+      <x:c r="A127" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="B127" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C127" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128">
+      <x:c r="A128" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="B128" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C128" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129">
+      <x:c r="A129" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B129" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C129" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130">
+      <x:c r="A130" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="B130" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C130" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131">
+      <x:c r="A131" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B131" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C131" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132">
+      <x:c r="A132" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B132" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C132" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133">
+      <x:c r="A133" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B133" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C133" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134">
+      <x:c r="A134" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="B134" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C134" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135">
+      <x:c r="A135" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B135" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C135" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136">
+      <x:c r="A136" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="B136" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C136" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137">
+      <x:c r="A137" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B137" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C137" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="138">
+      <x:c r="A138" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="B138" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C138" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139">
+      <x:c r="A139" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B139" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C139" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140">
+      <x:c r="A140" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="B140" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C140" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141">
+      <x:c r="A141" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="B141" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C141" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142">
+      <x:c r="A142" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="B142" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C142" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143">
+      <x:c r="A143" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B143" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C143" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144">
+      <x:c r="A144" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="B144" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C144" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145">
+      <x:c r="A145" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="B145" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C145" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146">
+      <x:c r="A146" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="B146" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C146" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147">
+      <x:c r="A147" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="B147" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C147" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148">
+      <x:c r="A148" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="B148" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C148" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149">
+      <x:c r="A149" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="B149" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C149" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150">
+      <x:c r="A150" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="B150" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C150" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151">
+      <x:c r="A151" t="s">
+        <x:v>156</x:v>
+      </x:c>
+      <x:c r="B151" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C151" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="152">
+      <x:c r="A152" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B152" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C152" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="153">
+      <x:c r="A153" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B153" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C153" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="154">
+      <x:c r="A154" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="B154" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C154" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155">
+      <x:c r="A155" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="B155" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C155" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156">
+      <x:c r="A156" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="B156" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C156" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157">
+      <x:c r="A157" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="B157" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C157" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158">
+      <x:c r="A158" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="B158" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C158" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159">
+      <x:c r="A159" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B159" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C159" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="160">
+      <x:c r="A160" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="B160" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C160" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>

</xml_diff>

<commit_message>
alert message for invalid file type
</commit_message>
<xml_diff>
--- a/TcpServer/bin/Debug/net8.0/logs.xlsx
+++ b/TcpServer/bin/Debug/net8.0/logs.xlsx
@@ -723,6 +723,33 @@
   </x:si>
   <x:si>
     <x:t>2024 March 29 9:06:25 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:09:59 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:10:04 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:10:18 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:11:09 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Image Signal Recieved</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:11:11 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:12:40 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:12:46 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 29 9:12:55 AM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3545,6 +3572,94 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
+    <x:row r="223">
+      <x:c r="A223" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="B223" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C223" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="224">
+      <x:c r="A224" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="B224" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C224" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="225">
+      <x:c r="A225" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="B225" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C225" t="s">
+        <x:v>131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="226">
+      <x:c r="A226" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="B226" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C226" t="s">
+        <x:v>233</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="227">
+      <x:c r="A227" t="s">
+        <x:v>234</x:v>
+      </x:c>
+      <x:c r="B227" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C227" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="228">
+      <x:c r="A228" t="s">
+        <x:v>235</x:v>
+      </x:c>
+      <x:c r="B228" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C228" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="229">
+      <x:c r="A229" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="B229" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C229" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="230">
+      <x:c r="A230" t="s">
+        <x:v>237</x:v>
+      </x:c>
+      <x:c r="B230" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C230" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>

</xml_diff>

<commit_message>
clean post for demo
</commit_message>
<xml_diff>
--- a/TcpServer/bin/Debug/net8.0/logs.xlsx
+++ b/TcpServer/bin/Debug/net8.0/logs.xlsx
@@ -300,6 +300,102 @@
   </x:si>
   <x:si>
     <x:t>5a6e39c9-fea6-4633-9011-4ecaa55aec2e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:06:40 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:06:42 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:09:13 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:09:23 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:09:25 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:10:26 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:10:33 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:10:34 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:10:43 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>68608f85-c49f-4034-95de-37af1d00386c</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:12:20 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:12:21 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:12:28 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>e22a62e1-95b9-40bb-98a2-c29a49478909</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:13:15 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>250d55b3-fb0f-476f-b4a7-c3f5e66f45c0.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:13:16 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Post Signal Recieved</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:19:12 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:20:36 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:20:37 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:20:47 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0cbf67f2-3871-4fdd-b377-cadd083f7f0f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:21:03 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>da7c2a43-fb79-4d15-a426-352033896b3b.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:21:04 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:31:33 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:31:34 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:31:42 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1d247121-e17d-44b3-9449-4f70318c9aaa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:32:48 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>910beebc-5e73-4088-b762-e0ce823111a5.jpg</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1362,6 +1458,281 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
+    <x:row r="63">
+      <x:c r="A63" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B63" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C63" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64">
+      <x:c r="A64" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B64" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C64" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65">
+      <x:c r="A65" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B65" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C65" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66">
+      <x:c r="A66" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B66" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C66" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67">
+      <x:c r="A67" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B67" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C67" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68">
+      <x:c r="A68" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B68" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C68" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69">
+      <x:c r="A69" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B69" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C69" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70">
+      <x:c r="A70" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B70" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C70" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71">
+      <x:c r="A71" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B71" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="C71" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72">
+      <x:c r="A72" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B72" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C72" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73">
+      <x:c r="A73" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B73" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C73" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74">
+      <x:c r="A74" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B74" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C74" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75">
+      <x:c r="A75" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B75" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="C75" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76">
+      <x:c r="A76" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B76" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C76" t="s">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77">
+      <x:c r="A77" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B77" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C77" t="s">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78">
+      <x:c r="A78" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B78" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C78" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79">
+      <x:c r="A79" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B79" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C79" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80">
+      <x:c r="A80" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B80" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="C80" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81">
+      <x:c r="A81" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="B81" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="C81" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82">
+      <x:c r="A82" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="B82" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="C82" t="s">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83">
+      <x:c r="A83" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="B83" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C83" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84">
+      <x:c r="A84" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="B84" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C84" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85">
+      <x:c r="A85" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="B85" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="C85" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86">
+      <x:c r="A86" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B86" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="C86" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87">
+      <x:c r="A87" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="B87" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="C87" t="s">
+        <x:v>105</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>

</xml_diff>

<commit_message>
fixed for issue 43
</commit_message>
<xml_diff>
--- a/TcpServer/bin/Debug/net8.0/logs.xlsx
+++ b/TcpServer/bin/Debug/net8.0/logs.xlsx
@@ -411,6 +411,12 @@
   </x:si>
   <x:si>
     <x:t>2024 March 31 4:37:07 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:42:09 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 4:42:10 AM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1792,6 +1798,28 @@
         <x:v>105</x:v>
       </x:c>
     </x:row>
+    <x:row r="92">
+      <x:c r="A92" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="B92" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C92" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93">
+      <x:c r="A93" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="B93" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C93" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>

</xml_diff>

<commit_message>
Added another dynamic test for pictures
</commit_message>
<xml_diff>
--- a/TcpServer/bin/Debug/net8.0/logs.xlsx
+++ b/TcpServer/bin/Debug/net8.0/logs.xlsx
@@ -438,6 +438,27 @@
   </x:si>
   <x:si>
     <x:t>2024 March 31 5:15:41 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 8:01:36 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 8:01:39 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 8:03:09 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 8:03:12 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 8:04:04 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>821c10dd-74d9-4802-ae40-a62040fda038</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 March 31 8:05:45 AM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1907,6 +1928,72 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
+    <x:row r="100">
+      <x:c r="A100" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="B100" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C100" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101">
+      <x:c r="A101" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="B101" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C101" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102">
+      <x:c r="A102" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="B102" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C102" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103">
+      <x:c r="A103" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B103" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C103" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104">
+      <x:c r="A104" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B104" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="C104" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105">
+      <x:c r="A105" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B105" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="C105" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>

</xml_diff>